<commit_message>
prototype sql parsing (select command)
</commit_message>
<xml_diff>
--- a/state_table.xlsx
+++ b/state_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasonw\Documents\Github\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Files\Github\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E5F8940-38FD-485A-8443-875A6C921E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3224EBA-3567-42DF-9A13-7FA29337B00A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="7448" xr2:uid="{72297823-02A6-44B6-B6AE-E6338D64CD0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72297823-02A6-44B6-B6AE-E6338D64CD0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,20 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>success?</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>comma</t>
   </si>
   <si>
@@ -81,6 +72,27 @@
   </si>
   <si>
     <t>VALUES</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>what to do with the last token?</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parse_tree["command"] = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">parse_tree["fields"] += </t>
+  </si>
+  <si>
+    <t>parse_tree["table_name"] =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parse_tree["where"] += </t>
   </si>
 </sst>
 </file>
@@ -480,72 +492,74 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.06640625" customWidth="1"/>
-    <col min="10" max="10" width="10.86328125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.86328125" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" s="4">
         <v>0</v>
       </c>
@@ -573,8 +587,10 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -600,8 +616,10 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -625,8 +643,10 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -652,7 +672,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>4</v>
@@ -677,7 +697,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <v>5</v>
@@ -702,8 +722,10 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -729,7 +751,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4">
         <v>7</v>
@@ -754,7 +776,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4">
         <v>8</v>
@@ -779,8 +801,10 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B11" s="4">
         <v>9</v>
       </c>
@@ -804,8 +828,10 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A12" s="4"/>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -829,8 +855,10 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B13" s="4">
         <v>11</v>
       </c>
@@ -852,8 +880,10 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -877,7 +907,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4">
         <v>13</v>
@@ -902,8 +932,10 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -927,7 +959,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4">
         <v>15</v>
@@ -952,8 +984,10 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B18" s="4">
         <v>16</v>
       </c>
@@ -979,7 +1013,7 @@
       </c>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4">
         <v>17</v>
@@ -1002,8 +1036,10 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B20" s="4">
         <v>18</v>
       </c>
@@ -1027,7 +1063,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4">
         <v>19</v>
@@ -1052,8 +1088,10 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B22" s="4">
         <v>20</v>
       </c>
@@ -1077,7 +1115,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4">
         <v>21</v>
@@ -1102,7 +1140,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4">
         <v>22</v>
@@ -1129,7 +1167,7 @@
       </c>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4">
         <v>23</v>
@@ -1154,7 +1192,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4">
         <v>24</v>
@@ -1179,7 +1217,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4">
         <v>25</v>
@@ -1204,7 +1242,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4">
         <v>26</v>
@@ -1231,7 +1269,7 @@
       </c>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4">
         <v>27</v>
@@ -1256,7 +1294,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4">
         <v>28</v>

</xml_diff>

<commit_message>
not sure what hanged here tbh
</commit_message>
<xml_diff>
--- a/state_table.xlsx
+++ b/state_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Files\Github\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D0ABBD-8206-4416-A5A0-480783798029}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C35CD8-7E5B-462C-A663-44AB7EE7FCFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="13800" windowHeight="9555" xr2:uid="{72297823-02A6-44B6-B6AE-E6338D64CD0B}"/>
+    <workbookView xWindow="3375" yWindow="1245" windowWidth="21705" windowHeight="13170" xr2:uid="{72297823-02A6-44B6-B6AE-E6338D64CD0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -502,21 +502,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AEEB66-474A-4971-8C7F-9B9936EF1DD2}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="O1" activeCellId="1" sqref="B22:O22 O1:O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.3984375" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="10" max="10" width="10.86328125" customWidth="1"/>
-    <col min="12" max="12" width="11.73046875" customWidth="1"/>
-    <col min="14" max="14" width="9.86328125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -572,7 +572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>0</v>
@@ -602,7 +602,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -632,7 +632,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -660,7 +660,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -690,7 +690,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2">
         <v>4</v>
@@ -716,7 +716,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2">
         <v>5</v>
@@ -742,7 +742,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2">
         <v>7</v>
@@ -798,7 +798,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2">
         <v>8</v>
@@ -824,7 +824,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -880,7 +880,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -908,7 +908,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -936,7 +936,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2">
         <v>14</v>
@@ -990,7 +990,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1018,7 +1018,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2">
         <v>16</v>
@@ -1044,7 +1044,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2">
         <v>18</v>
@@ -1100,7 +1100,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>19</v>
       </c>
@@ -1123,7 +1123,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2">
         <v>22</v>
@@ -1205,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2">
         <v>23</v>
@@ -1231,7 +1231,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2">
         <v>24</v>
@@ -1259,7 +1259,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
         <v>25</v>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2">
         <v>26</v>
@@ -1313,7 +1313,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2">
         <v>27</v>
@@ -1337,7 +1337,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2">
         <v>28</v>
@@ -1361,7 +1361,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2">
         <v>29</v>
@@ -1385,7 +1385,7 @@
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2">
         <v>30</v>

</xml_diff>

<commit_message>
ignore weird commit typo
</commit_message>
<xml_diff>
--- a/state_table.xlsx
+++ b/state_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Files\Github\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C35CD8-7E5B-462C-A663-44AB7EE7FCFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353B8DFF-B38F-4A13-8F27-6D96D582A4C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3375" yWindow="1245" windowWidth="21705" windowHeight="13170" xr2:uid="{72297823-02A6-44B6-B6AE-E6338D64CD0B}"/>
   </bookViews>
@@ -502,21 +502,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AEEB66-474A-4971-8C7F-9B9936EF1DD2}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="O1" activeCellId="1" sqref="B22:O22 O1:O22"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="90" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.3984375" customWidth="1"/>
+    <col min="4" max="4" width="10.265625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.86328125" customWidth="1"/>
+    <col min="12" max="12" width="11.73046875" customWidth="1"/>
+    <col min="14" max="14" width="9.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -572,7 +572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>0</v>
@@ -602,7 +602,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -632,7 +632,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -660,7 +660,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -690,7 +690,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2">
         <v>4</v>
@@ -716,7 +716,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="2">
         <v>5</v>
@@ -742,7 +742,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="2">
         <v>7</v>
@@ -798,7 +798,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
       <c r="B10" s="2">
         <v>8</v>
@@ -824,7 +824,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -880,7 +880,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -908,7 +908,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -936,7 +936,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="2">
         <v>14</v>
@@ -990,7 +990,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1018,7 +1018,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
       <c r="B18" s="2">
         <v>16</v>
@@ -1044,7 +1044,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="2">
         <v>18</v>
@@ -1100,7 +1100,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B21" s="2">
         <v>19</v>
       </c>
@@ -1123,7 +1123,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="2">
         <v>22</v>
@@ -1205,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="2">
         <v>23</v>
@@ -1231,7 +1231,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="2">
         <v>24</v>
@@ -1259,7 +1259,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
         <v>25</v>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="2">
         <v>26</v>
@@ -1313,7 +1313,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="2">
         <v>27</v>
@@ -1337,7 +1337,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="2">
         <v>28</v>
@@ -1361,7 +1361,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
       <c r="B31" s="2">
         <v>29</v>
@@ -1385,7 +1385,7 @@
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="2">
         <v>30</v>

</xml_diff>